<commit_message>
NÅ FUNKER DET BRA HER  - god helg :)
</commit_message>
<xml_diff>
--- a/Old Model/Input/model_input_9groups_2or3spec.xlsx
+++ b/Old Model/Input/model_input_9groups_2or3spec.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oyvindasplin/Documents/Indok/NTNU/Optimering/Master V22/master2022/Old Model/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29A2E61D-C22C-954A-8180-7650E8AFE966}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A17D8E-F029-1B49-94BE-F09278FAF8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="500" windowWidth="38400" windowHeight="19260" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19260" activeTab="3" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="14" r:id="rId1"/>
@@ -1120,7 +1120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1975E0D-6F6E-A842-BF84-34A209557AB1}">
   <dimension ref="A1:DG61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="U6" sqref="U6"/>
     </sheetView>
   </sheetViews>
@@ -5800,8 +5800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B305B3B2-E098-F04C-83CE-B18CE5C01F35}">
   <dimension ref="A1:AS32"/>
   <sheetViews>
-    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6515,10 +6515,10 @@
         <v>42</v>
       </c>
       <c r="B9" s="53">
-        <v>4.2622950819672129E-2</v>
+        <v>0.91304347826086951</v>
       </c>
       <c r="C9" s="54">
-        <v>2.4590163934426229E-2</v>
+        <v>0.52173913043478259</v>
       </c>
       <c r="D9" s="54">
         <v>0</v>
@@ -6603,10 +6603,10 @@
         <v>41</v>
       </c>
       <c r="B10" s="56">
-        <v>0.91304347826086951</v>
+        <v>4.2622950819672129E-2</v>
       </c>
       <c r="C10" s="57">
-        <v>0.52173913043478259</v>
+        <v>2.4590163934426229E-2</v>
       </c>
       <c r="D10" s="57">
         <v>0</v>
@@ -7213,6 +7213,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010014502AD36FC4D1459EE8BFEB917118AE" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="4b4cd19ef6f825a6ac181b2aef79b604">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1a062c2-eeb0-45d1-8c80-71eb2bb91349" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="944c6668d3530cb8510fee0a023b67da" ns2:_="">
     <xsd:import namespace="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
@@ -7384,12 +7390,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6800F54-1DFB-4342-B9AD-C5A078244FA9}">
   <ds:schemaRefs>
@@ -7399,6 +7399,22 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C068943E-AD27-4D1A-99C2-3677F095010F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C770A5B5-1066-461F-A7CC-945216CB7576}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7414,20 +7430,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C068943E-AD27-4D1A-99C2-3677F095010F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="a1a062c2-eeb0-45d1-8c80-71eb2bb91349"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Masse endringer i patterns og slettede Excel-filer
</commit_message>
<xml_diff>
--- a/Old Model/Input/model_input_9groups_2or3spec.xlsx
+++ b/Old Model/Input/model_input_9groups_2or3spec.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10111"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/oyvindasplin/Documents/Indok/NTNU/Optimering/Master V22/master2022/Old Model/Input/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/katarinavandepontseele/Documents/Skole/10semester/master2022/Old Model/Input/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0A17D8E-F029-1B49-94BE-F09278FAF8D7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CB046C8-F76D-974D-A205-04E8845C6240}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19260" activeTab="3" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{A5361B1D-8409-0845-981B-BA630B7E70E6}"/>
   </bookViews>
   <sheets>
     <sheet name="Parameters" sheetId="14" r:id="rId1"/>
@@ -802,9 +802,9 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="20% - Accent4" xfId="1" builtinId="42"/>
-    <cellStyle name="20% - Accent5" xfId="3" builtinId="46"/>
-    <cellStyle name="20% - Accent6" xfId="4" builtinId="50"/>
+    <cellStyle name="20 % – uthevingsfarge 4" xfId="1" builtinId="42"/>
+    <cellStyle name="20 % – uthevingsfarge 5" xfId="3" builtinId="46"/>
+    <cellStyle name="20 % – uthevingsfarge 6" xfId="4" builtinId="50"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="2" xr:uid="{8F977E11-39D4-E04C-8D51-A4F1FE1B59AD}"/>
   </cellStyles>
@@ -822,7 +822,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1120,8 +1120,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1975E0D-6F6E-A842-BF84-34A209557AB1}">
   <dimension ref="A1:DG61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U6" sqref="U6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5800,7 +5800,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B305B3B2-E098-F04C-83CE-B18CE5C01F35}">
   <dimension ref="A1:AS32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
@@ -7204,18 +7204,18 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7391,14 +7391,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6800F54-1DFB-4342-B9AD-C5A078244FA9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C068943E-AD27-4D1A-99C2-3677F095010F}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
@@ -7410,6 +7402,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E6800F54-1DFB-4342-B9AD-C5A078244FA9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>